<commit_message>
fix error with file names
</commit_message>
<xml_diff>
--- a/core.xlsx
+++ b/core.xlsx
@@ -9,23 +9,119 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Число</t>
-  </si>
-  <si>
-    <t>Ожидаемый результат</t>
-  </si>
-  <si>
-    <t>один миллион двенадцать тысяч три</t>
-  </si>
-  <si>
-    <t>тринадцать миллионов четыреста четырнадцать тысяч триста девяносто девять</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>один</t>
+  </si>
+  <si>
+    <t>два</t>
+  </si>
+  <si>
+    <t>три</t>
+  </si>
+  <si>
+    <t>четыре</t>
+  </si>
+  <si>
+    <t>пять</t>
+  </si>
+  <si>
+    <t>шесть</t>
+  </si>
+  <si>
+    <t>семь</t>
+  </si>
+  <si>
+    <t>восемь</t>
+  </si>
+  <si>
+    <t>девять</t>
+  </si>
+  <si>
+    <t>десять</t>
+  </si>
+  <si>
+    <t>двенадцать</t>
+  </si>
+  <si>
+    <t>тринадцать</t>
+  </si>
+  <si>
+    <t>четырнадцать</t>
+  </si>
+  <si>
+    <t>пятнадцать</t>
+  </si>
+  <si>
+    <t>шестнадцать</t>
+  </si>
+  <si>
+    <t>восемнадцать</t>
+  </si>
+  <si>
+    <t>семнадцать</t>
+  </si>
+  <si>
+    <t>девятнадцать</t>
+  </si>
+  <si>
+    <t>двадцать</t>
+  </si>
+  <si>
+    <t>сорок</t>
+  </si>
+  <si>
+    <t>сто</t>
+  </si>
+  <si>
+    <t>тридцать</t>
+  </si>
+  <si>
+    <t>пятьдясят</t>
+  </si>
+  <si>
+    <t>шестьдесят</t>
+  </si>
+  <si>
+    <t>двесте</t>
+  </si>
+  <si>
+    <t>триста</t>
+  </si>
+  <si>
+    <t>пятьсот</t>
+  </si>
+  <si>
+    <t>шестьсот</t>
+  </si>
+  <si>
+    <t>девятьсот</t>
+  </si>
+  <si>
+    <t>одиннадцать</t>
+  </si>
+  <si>
+    <t>восемьдесят</t>
+  </si>
+  <si>
+    <t>семьдесят</t>
+  </si>
+  <si>
+    <t>девяносто</t>
+  </si>
+  <si>
+    <t>четыреста</t>
+  </si>
+  <si>
+    <t>семьсот</t>
+  </si>
+  <si>
+    <t>восемьсот</t>
   </si>
 </sst>
 </file>
@@ -367,41 +463,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="65.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1012003</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>13414399</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>200</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>300</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>400</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>500</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>600</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>700</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>800</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>900</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>